<commit_message>
Working till now to be work on attack path
</commit_message>
<xml_diff>
--- a/New folder/triaging_template_Rule_014-New User Assigned to Privileged Role.xlsx
+++ b/New folder/triaging_template_Rule_014-New User Assigned to Privileged Role.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agentic AI\Projects\soc\triaging_template\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4A8906-3440-403F-8095-42D82C77D965}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01435063-1175-4F92-866A-259C31436F6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,17 +711,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="61.109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
   </cols>
   <sheetData>
@@ -798,7 +798,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="360" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A11" si="0">A4+1</f>
         <v>3</v>

</xml_diff>